<commit_message>
Limpieza de datos: corregidos errores de encoding y generados reportes
</commit_message>
<xml_diff>
--- a/Reportes/reporte_faltantes.xlsx
+++ b/Reportes/reporte_faltantes.xlsx
@@ -457,10 +457,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3928</v>
+        <v>3925</v>
       </c>
       <c r="C2" t="n">
-        <v>61.15522341584929</v>
+        <v>61.13707165109034</v>
       </c>
     </row>
     <row r="3">
@@ -470,10 +470,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3808</v>
+        <v>3807</v>
       </c>
       <c r="C3" t="n">
-        <v>59.28693756811458</v>
+        <v>59.29906542056075</v>
       </c>
     </row>
     <row r="4">
@@ -483,10 +483,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3217</v>
+        <v>3214</v>
       </c>
       <c r="C4" t="n">
-        <v>50.08562976802118</v>
+        <v>50.06230529595016</v>
       </c>
     </row>
     <row r="5">
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3200</v>
+        <v>3197</v>
       </c>
       <c r="C5" t="n">
-        <v>49.8209559395921</v>
+        <v>49.79750778816199</v>
       </c>
     </row>
     <row r="6">
@@ -512,7 +512,7 @@
         <v>1939</v>
       </c>
       <c r="C6" t="n">
-        <v>30.18838548964658</v>
+        <v>30.20249221183801</v>
       </c>
     </row>
     <row r="7">
@@ -525,7 +525,7 @@
         <v>1939</v>
       </c>
       <c r="C7" t="n">
-        <v>30.18838548964658</v>
+        <v>30.20249221183801</v>
       </c>
     </row>
     <row r="8">
@@ -538,7 +538,7 @@
         <v>889</v>
       </c>
       <c r="C8" t="n">
-        <v>13.84088432196793</v>
+        <v>13.84735202492212</v>
       </c>
     </row>
     <row r="9">
@@ -551,7 +551,7 @@
         <v>885</v>
       </c>
       <c r="C9" t="n">
-        <v>13.77860812704344</v>
+        <v>13.78504672897196</v>
       </c>
     </row>
     <row r="10">
@@ -564,7 +564,7 @@
         <v>13</v>
       </c>
       <c r="C10" t="n">
-        <v>0.2023976335045929</v>
+        <v>0.2024922118380063</v>
       </c>
     </row>
     <row r="11">
@@ -577,7 +577,7 @@
         <v>13</v>
       </c>
       <c r="C11" t="n">
-        <v>0.2023976335045929</v>
+        <v>0.2024922118380063</v>
       </c>
     </row>
     <row r="12">

</xml_diff>